<commit_message>
corrigindo detalhes das instruções para gerar corretamente as tabelas
</commit_message>
<xml_diff>
--- a/isa_instmem.xlsx
+++ b/isa_instmem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\5o ANO ELO\ARQ COMP\logisim\MicroprocMIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E06E89E4-E79E-4489-8663-65892518BD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A7DC44-FB19-4FC5-95BA-B65D5081B8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4875" windowWidth="29040" windowHeight="15720" xr2:uid="{6C5198ED-5DFF-4969-B60C-5EFD2EF9DAE2}"/>
+    <workbookView xWindow="34785" yWindow="-4755" windowWidth="14610" windowHeight="15585" xr2:uid="{6C5198ED-5DFF-4969-B60C-5EFD2EF9DAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -518,31 +518,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -561,27 +582,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -900,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C09B202-C78D-42EA-8D8A-A90EDC4212BD}">
   <dimension ref="A1:AR34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,27 +1086,27 @@
       <c r="Q2" s="10">
         <v>0</v>
       </c>
-      <c r="R2" s="55" t="s">
+      <c r="R2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="55" t="s">
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="58" t="s">
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="AC2" s="58"/>
-      <c r="AD2" s="58"/>
-      <c r="AE2" s="58"/>
-      <c r="AF2" s="58"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
       <c r="AG2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1178,27 +1178,27 @@
       <c r="Q3" s="12">
         <v>0</v>
       </c>
-      <c r="R3" s="53" t="s">
+      <c r="R3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="53" t="s">
+      <c r="S3" s="45"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="38" t="s">
+      <c r="X3" s="45"/>
+      <c r="Y3" s="45"/>
+      <c r="Z3" s="45"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="AC3" s="38"/>
-      <c r="AD3" s="38"/>
-      <c r="AE3" s="38"/>
-      <c r="AF3" s="38"/>
+      <c r="AC3" s="45"/>
+      <c r="AD3" s="45"/>
+      <c r="AE3" s="45"/>
+      <c r="AF3" s="45"/>
       <c r="AG3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1273,27 +1273,27 @@
       <c r="Q4" s="12">
         <v>0</v>
       </c>
-      <c r="R4" s="53" t="s">
+      <c r="R4" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="54"/>
-      <c r="W4" s="53" t="s">
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="54"/>
-      <c r="AB4" s="38" t="s">
+      <c r="X4" s="45"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="46"/>
+      <c r="AB4" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="38"/>
-      <c r="AE4" s="38"/>
-      <c r="AF4" s="38"/>
+      <c r="AC4" s="45"/>
+      <c r="AD4" s="45"/>
+      <c r="AE4" s="45"/>
+      <c r="AF4" s="45"/>
       <c r="AG4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1368,27 +1368,27 @@
       <c r="Q5" s="12">
         <v>0</v>
       </c>
-      <c r="R5" s="53" t="s">
+      <c r="R5" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="54"/>
-      <c r="W5" s="53" t="s">
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="38" t="s">
+      <c r="X5" s="45"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="45"/>
+      <c r="AA5" s="46"/>
+      <c r="AB5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="38"/>
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="45"/>
       <c r="AG5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1457,38 +1457,38 @@
       <c r="Q6" s="12">
         <v>1</v>
       </c>
-      <c r="R6" s="41" t="s">
+      <c r="R6" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="44" t="s">
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="46"/>
-      <c r="AB6" s="40" t="s">
+      <c r="X6" s="51"/>
+      <c r="Y6" s="51"/>
+      <c r="Z6" s="51"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="40"/>
-      <c r="AD6" s="40"/>
-      <c r="AE6" s="40"/>
-      <c r="AF6" s="40"/>
-      <c r="AG6" s="40"/>
-      <c r="AH6" s="40"/>
-      <c r="AI6" s="40"/>
-      <c r="AJ6" s="40"/>
-      <c r="AK6" s="40"/>
-      <c r="AL6" s="40"/>
-      <c r="AM6" s="40"/>
-      <c r="AN6" s="40"/>
-      <c r="AO6" s="40"/>
-      <c r="AP6" s="40"/>
-      <c r="AQ6" s="40"/>
+      <c r="AC6" s="53"/>
+      <c r="AD6" s="53"/>
+      <c r="AE6" s="53"/>
+      <c r="AF6" s="53"/>
+      <c r="AG6" s="53"/>
+      <c r="AH6" s="53"/>
+      <c r="AI6" s="53"/>
+      <c r="AJ6" s="53"/>
+      <c r="AK6" s="53"/>
+      <c r="AL6" s="53"/>
+      <c r="AM6" s="53"/>
+      <c r="AN6" s="53"/>
+      <c r="AO6" s="53"/>
+      <c r="AP6" s="53"/>
+      <c r="AQ6" s="53"/>
       <c r="AR6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1518,38 +1518,38 @@
       <c r="Q7" s="12">
         <v>1</v>
       </c>
-      <c r="R7" s="41" t="s">
+      <c r="R7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="42"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="44" t="s">
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="46"/>
-      <c r="AB7" s="40" t="s">
+      <c r="X7" s="51"/>
+      <c r="Y7" s="51"/>
+      <c r="Z7" s="51"/>
+      <c r="AA7" s="52"/>
+      <c r="AB7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="AC7" s="40"/>
-      <c r="AD7" s="40"/>
-      <c r="AE7" s="40"/>
-      <c r="AF7" s="40"/>
-      <c r="AG7" s="40"/>
-      <c r="AH7" s="40"/>
-      <c r="AI7" s="40"/>
-      <c r="AJ7" s="40"/>
-      <c r="AK7" s="40"/>
-      <c r="AL7" s="40"/>
-      <c r="AM7" s="40"/>
-      <c r="AN7" s="40"/>
-      <c r="AO7" s="40"/>
-      <c r="AP7" s="40"/>
-      <c r="AQ7" s="40"/>
+      <c r="AC7" s="53"/>
+      <c r="AD7" s="53"/>
+      <c r="AE7" s="53"/>
+      <c r="AF7" s="53"/>
+      <c r="AG7" s="53"/>
+      <c r="AH7" s="53"/>
+      <c r="AI7" s="53"/>
+      <c r="AJ7" s="53"/>
+      <c r="AK7" s="53"/>
+      <c r="AL7" s="53"/>
+      <c r="AM7" s="53"/>
+      <c r="AN7" s="53"/>
+      <c r="AO7" s="53"/>
+      <c r="AP7" s="53"/>
+      <c r="AQ7" s="53"/>
       <c r="AR7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1579,38 +1579,38 @@
       <c r="Q8" s="14">
         <v>0</v>
       </c>
-      <c r="R8" s="47" t="s">
+      <c r="R8" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="49"/>
-      <c r="W8" s="50" t="s">
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
+      <c r="V8" s="56"/>
+      <c r="W8" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="51"/>
-      <c r="Z8" s="51"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="39" t="s">
+      <c r="X8" s="58"/>
+      <c r="Y8" s="58"/>
+      <c r="Z8" s="58"/>
+      <c r="AA8" s="59"/>
+      <c r="AB8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="39"/>
-      <c r="AD8" s="39"/>
-      <c r="AE8" s="39"/>
-      <c r="AF8" s="39"/>
-      <c r="AG8" s="39"/>
-      <c r="AH8" s="39"/>
-      <c r="AI8" s="39"/>
-      <c r="AJ8" s="39"/>
-      <c r="AK8" s="39"/>
-      <c r="AL8" s="39"/>
-      <c r="AM8" s="39"/>
-      <c r="AN8" s="39"/>
-      <c r="AO8" s="39"/>
-      <c r="AP8" s="39"/>
-      <c r="AQ8" s="39"/>
+      <c r="AC8" s="43"/>
+      <c r="AD8" s="43"/>
+      <c r="AE8" s="43"/>
+      <c r="AF8" s="43"/>
+      <c r="AG8" s="43"/>
+      <c r="AH8" s="43"/>
+      <c r="AI8" s="43"/>
+      <c r="AJ8" s="43"/>
+      <c r="AK8" s="43"/>
+      <c r="AL8" s="43"/>
+      <c r="AM8" s="43"/>
+      <c r="AN8" s="43"/>
+      <c r="AO8" s="43"/>
+      <c r="AP8" s="43"/>
+      <c r="AQ8" s="43"/>
       <c r="AR8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1667,24 +1667,24 @@
       <c r="AA9" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="AB9" s="59" t="s">
+      <c r="AB9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="AC9" s="39"/>
-      <c r="AD9" s="39"/>
-      <c r="AE9" s="39"/>
-      <c r="AF9" s="39"/>
-      <c r="AG9" s="39"/>
-      <c r="AH9" s="39"/>
-      <c r="AI9" s="39"/>
-      <c r="AJ9" s="39"/>
-      <c r="AK9" s="39"/>
-      <c r="AL9" s="39"/>
-      <c r="AM9" s="39"/>
-      <c r="AN9" s="39"/>
-      <c r="AO9" s="39"/>
-      <c r="AP9" s="39"/>
-      <c r="AQ9" s="39"/>
+      <c r="AC9" s="43"/>
+      <c r="AD9" s="43"/>
+      <c r="AE9" s="43"/>
+      <c r="AF9" s="43"/>
+      <c r="AG9" s="43"/>
+      <c r="AH9" s="43"/>
+      <c r="AI9" s="43"/>
+      <c r="AJ9" s="43"/>
+      <c r="AK9" s="43"/>
+      <c r="AL9" s="43"/>
+      <c r="AM9" s="43"/>
+      <c r="AN9" s="43"/>
+      <c r="AO9" s="43"/>
+      <c r="AP9" s="43"/>
+      <c r="AQ9" s="43"/>
       <c r="AR9" s="3"/>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
@@ -1722,12 +1722,12 @@
       <c r="D12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
       <c r="I12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1850,12 +1850,12 @@
       <c r="D13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
       <c r="I13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1978,12 +1978,12 @@
       <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="1" t="s">
         <v>35</v>
       </c>
@@ -2103,12 +2103,12 @@
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
       <c r="K15" s="1" t="s">
         <v>36</v>
       </c>
@@ -2225,12 +2225,12 @@
       <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
       <c r="K16" s="1" t="s">
         <v>37</v>
       </c>
@@ -2347,12 +2347,12 @@
       <c r="D17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
       <c r="I17" s="37"/>
       <c r="K17" s="1" t="s">
         <v>38</v>
@@ -2571,12 +2571,12 @@
       </c>
     </row>
     <row r="20" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="E20" s="38" t="s">
+      <c r="E20" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
       <c r="I20" s="1" t="s">
         <v>23</v>
       </c>
@@ -2594,12 +2594,12 @@
       </c>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="1" t="s">
         <v>24</v>
       </c>
@@ -2618,12 +2618,12 @@
       <c r="R21" s="37"/>
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
       <c r="I22" s="1" t="s">
         <v>29</v>
       </c>
@@ -2643,12 +2643,12 @@
       <c r="R22" s="37"/>
     </row>
     <row r="23" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
       <c r="L23" s="1" t="s">
         <v>60</v>
       </c>
@@ -2657,12 +2657,12 @@
       </c>
     </row>
     <row r="24" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
       <c r="I24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2680,12 +2680,12 @@
       </c>
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
       <c r="I25" s="1" t="s">
         <v>50</v>
       </c>
@@ -2767,6 +2767,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="AB8:AQ8"/>
+    <mergeCell ref="AB6:AQ6"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="R8:V8"/>
+    <mergeCell ref="W8:AA8"/>
     <mergeCell ref="R2:V2"/>
     <mergeCell ref="W2:AA2"/>
     <mergeCell ref="AB2:AF2"/>
@@ -2783,24 +2801,6 @@
     <mergeCell ref="R6:V6"/>
     <mergeCell ref="W6:AA6"/>
     <mergeCell ref="AB7:AQ7"/>
-    <mergeCell ref="AB6:AQ6"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="R8:V8"/>
-    <mergeCell ref="W8:AA8"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="AB8:AQ8"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>